<commit_message>
added candidate list option
</commit_message>
<xml_diff>
--- a/hospitals.xlsx
+++ b/hospitals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\enactus\matching_enactus_munich\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9887FC6-27C7-4848-97FA-C58B1C295A46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42D339D-91ED-4F1A-84B4-D94175EFDF84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{CE36E632-523C-4BA8-ACF3-1AC0E261F01D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -39,31 +39,22 @@
     <t>EduGlobe</t>
   </si>
   <si>
-    <t>FoodGrube</t>
-  </si>
-  <si>
-    <t>Glassic</t>
-  </si>
-  <si>
-    <t>ReStove</t>
-  </si>
-  <si>
     <t>SeaSoilution</t>
   </si>
   <si>
-    <t>Techdalo</t>
-  </si>
-  <si>
-    <t>Waterfilter</t>
-  </si>
-  <si>
     <t>Mistub</t>
   </si>
   <si>
-    <t>TownBee</t>
-  </si>
-  <si>
     <t>Capacities</t>
+  </si>
+  <si>
+    <t>Foodgrube</t>
+  </si>
+  <si>
+    <t>Townbee</t>
+  </si>
+  <si>
+    <t>Operations</t>
   </si>
 </sst>
 </file>
@@ -87,12 +78,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,9 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641E3B11-DA73-4891-BC1A-DFC8FED0465E}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -435,88 +435,60 @@
     <col min="1" max="1" width="10.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1">
-        <f>SUM(B2:B10)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
       <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>